<commit_message>
Final Commit. Add support of light and dark themes. Add support of ukrainian and english languages. Also fix some bugs.
</commit_message>
<xml_diff>
--- a/ProjectScheme.xlsx
+++ b/ProjectScheme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pc programs\ospanel\domains\raccoons-courses-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7403D1E5-F3AA-4C3E-BFC2-3C040C321485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1165E45-173C-4903-AC2F-C4C3150AE577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="517" xr2:uid="{F577DFC7-EC15-466B-9867-EE0FDB83E09B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>User</t>
   </si>
@@ -213,14 +213,50 @@
     <t>avatar</t>
   </si>
   <si>
-    <t>12.5%</t>
+    <t>Вывод карточки товара/категории на окне удаления товара/категории</t>
+  </si>
+  <si>
+    <t>Карточки будут с использованием классов бутстрапа</t>
+  </si>
+  <si>
+    <t>Прикрепить футер к нижней части экрана</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>dark theme folders</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>light theme folders</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +286,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -317,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -358,9 +403,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -378,6 +420,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1154,14 +1200,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B307AFD9-168D-4D30-9930-BE180DFB29B0}">
   <dimension ref="B4:S112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
@@ -1251,7 +1297,7 @@
       </c>
     </row>
     <row r="12" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="24" t="s">
         <v>56</v>
       </c>
       <c r="J12" s="3"/>
@@ -1400,10 +1446,10 @@
       <c r="I24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K24" s="24" t="s">
+      <c r="K24" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1455,7 +1501,7 @@
         <v>0.5</v>
       </c>
       <c r="E29" s="12"/>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="21" t="s">
         <v>31</v>
       </c>
       <c r="G29" s="15">
@@ -1463,29 +1509,29 @@
       </c>
     </row>
     <row r="30" spans="2:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="15">
         <v>1</v>
       </c>
       <c r="E30" s="12"/>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="14">
-        <v>0.5</v>
+      <c r="G30" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:19" ht="60" x14ac:dyDescent="0.25">
       <c r="C31" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="14">
-        <v>0.25</v>
+      <c r="D31" s="15">
+        <v>1</v>
       </c>
       <c r="E31" s="12"/>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G31" s="15">
@@ -1497,14 +1543,14 @@
         <v>55</v>
       </c>
       <c r="D32" s="14">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C33" s="19" t="s">
+    <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="15">
@@ -1514,8 +1560,8 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C34" s="19" t="s">
+    <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="15">
@@ -1525,20 +1571,20 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="3:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="22" t="s">
+    <row r="35" spans="2:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C36" s="11" t="s">
+    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>60</v>
+      <c r="D36" s="15">
+        <v>1</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>38</v>
@@ -1547,55 +1593,55 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="3:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C37" s="11" t="s">
+    <row r="37" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C37" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="14">
-        <v>0</v>
+      <c r="D37" s="15">
+        <v>1</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G37" s="21">
+      <c r="G37" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="11" t="s">
+    <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="14">
-        <v>0</v>
-      </c>
-      <c r="F38" s="22" t="s">
+      <c r="D38" s="15">
+        <v>1</v>
+      </c>
+      <c r="F38" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G38" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="F39" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="21">
+      <c r="G39" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="F40" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="F41" s="11" t="s">
         <v>49</v>
       </c>
@@ -1603,28 +1649,139 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="11"/>
-      <c r="G42" s="20"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F43" s="11"/>
-      <c r="G43" s="20"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="F42" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F43" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F44" s="11"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="54" spans="9:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="19"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="26">
+        <v>1</v>
+      </c>
+      <c r="D47" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="19">
+        <v>1</v>
+      </c>
+      <c r="D48" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="19">
+        <v>1</v>
+      </c>
+      <c r="D49" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="19">
+        <v>1</v>
+      </c>
+      <c r="D50" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="19">
+        <v>1</v>
+      </c>
+      <c r="D51" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="19">
+        <v>1</v>
+      </c>
+      <c r="D52" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="19">
+        <v>1</v>
+      </c>
+      <c r="D53" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
       <c r="I54" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
-      <c r="M54" t="s">
+      <c r="M54" s="25" t="s">
         <v>48</v>
       </c>
+      <c r="Q54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
     </row>
     <row r="83" spans="9:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I83" s="17" t="s">

</xml_diff>